<commit_message>
Added 72 index funds to prediction
</commit_message>
<xml_diff>
--- a/Stock_Market/ticker_list/ticker_list.xlsx
+++ b/Stock_Market/ticker_list/ticker_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Public_Github\Sentiment_Analysis\Stock_Market\ticker_list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE868B9D-6115-4FC4-A262-41A2EE0A65B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C95DFCE-72CF-4208-94E5-2C93EBB704A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="1668" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ticker_sheet" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="143">
   <si>
     <t>ticker_name</t>
   </si>
@@ -55,13 +55,412 @@
   </si>
   <si>
     <t>^DJI</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>EL</t>
+  </si>
+  <si>
+    <t>ARKK</t>
+  </si>
+  <si>
+    <t>ASML</t>
+  </si>
+  <si>
+    <t>STZ</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>HAL</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>DVN</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>AVGO</t>
+  </si>
+  <si>
+    <t>MRVL</t>
+  </si>
+  <si>
+    <t>DHR</t>
+  </si>
+  <si>
+    <t>ABBV</t>
+  </si>
+  <si>
+    <t>DIS</t>
+  </si>
+  <si>
+    <t>NUE</t>
+  </si>
+  <si>
+    <t>LLY</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>CVX</t>
+  </si>
+  <si>
+    <t>PYPL</t>
+  </si>
+  <si>
+    <t>RBLX</t>
+  </si>
+  <si>
+    <t>PATH</t>
+  </si>
+  <si>
+    <t>COST</t>
+  </si>
+  <si>
+    <t>ABNB</t>
+  </si>
+  <si>
+    <t>BGS</t>
+  </si>
+  <si>
+    <t>KMI</t>
+  </si>
+  <si>
+    <t>ETSY</t>
+  </si>
+  <si>
+    <t>NOW</t>
+  </si>
+  <si>
+    <t>OKTA</t>
+  </si>
+  <si>
+    <t>WMT</t>
+  </si>
+  <si>
+    <t>SNOW</t>
+  </si>
+  <si>
+    <t>SPLK</t>
+  </si>
+  <si>
+    <t>TDOC</t>
+  </si>
+  <si>
+    <t>CSCO</t>
+  </si>
+  <si>
+    <t>ORCL</t>
+  </si>
+  <si>
+    <t>HON</t>
+  </si>
+  <si>
+    <t>VZ</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>TSM</t>
+  </si>
+  <si>
+    <t>SHOP</t>
+  </si>
+  <si>
+    <t>PANW</t>
+  </si>
+  <si>
+    <t>TEAM</t>
+  </si>
+  <si>
+    <t>ADBE</t>
+  </si>
+  <si>
+    <t>CRWD</t>
+  </si>
+  <si>
+    <t>SWKS</t>
+  </si>
+  <si>
+    <t>LMND</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>SBUX</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>SQ</t>
+  </si>
+  <si>
+    <t>TSLA</t>
+  </si>
+  <si>
+    <t>QCOM</t>
+  </si>
+  <si>
+    <t>NVEC</t>
+  </si>
+  <si>
+    <t>NVDA</t>
+  </si>
+  <si>
+    <t>NFLX</t>
+  </si>
+  <si>
+    <t>JNJ</t>
+  </si>
+  <si>
+    <t>GOOG</t>
+  </si>
+  <si>
+    <t>META</t>
+  </si>
+  <si>
+    <t>BABA</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>AMZN</t>
+  </si>
+  <si>
+    <t>AAPL</t>
+  </si>
+  <si>
+    <t>EBAY</t>
+  </si>
+  <si>
+    <t>JPM</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>BIIB</t>
+  </si>
+  <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>MCHP</t>
+  </si>
+  <si>
+    <t>NKE</t>
+  </si>
+  <si>
+    <t>APPLE</t>
+  </si>
+  <si>
+    <t>ABBVIE</t>
+  </si>
+  <si>
+    <t>AIRBNB</t>
+  </si>
+  <si>
+    <t>ADOBE</t>
+  </si>
+  <si>
+    <t>AMAZON</t>
+  </si>
+  <si>
+    <t>ARK_INNOVATION</t>
+  </si>
+  <si>
+    <t>ASML_Holding</t>
+  </si>
+  <si>
+    <t>BROADCOM</t>
+  </si>
+  <si>
+    <t>BOEING</t>
+  </si>
+  <si>
+    <t>ALIBABA</t>
+  </si>
+  <si>
+    <t>BandG_Foods</t>
+  </si>
+  <si>
+    <t>Biogen</t>
+  </si>
+  <si>
+    <t>CATERPILLAR</t>
+  </si>
+  <si>
+    <t>COSTCO</t>
+  </si>
+  <si>
+    <t>SALESFORCE</t>
+  </si>
+  <si>
+    <t>CROWDSTRIKE</t>
+  </si>
+  <si>
+    <t>CISCO</t>
+  </si>
+  <si>
+    <t>CHEVRON</t>
+  </si>
+  <si>
+    <t>DANAHER</t>
+  </si>
+  <si>
+    <t>DISNEY</t>
+  </si>
+  <si>
+    <t>DEVON_ENERGY</t>
+  </si>
+  <si>
+    <t>ESTEE_LAUDER</t>
+  </si>
+  <si>
+    <t>GENERAL_ELECTRIC</t>
+  </si>
+  <si>
+    <t>GOOGLE</t>
+  </si>
+  <si>
+    <t>HALLIBURTON</t>
+  </si>
+  <si>
+    <t>HONEYWELL</t>
+  </si>
+  <si>
+    <t>JPMORGAN</t>
+  </si>
+  <si>
+    <t>KINDER_MORGAN</t>
+  </si>
+  <si>
+    <t>ELI_LILLY</t>
+  </si>
+  <si>
+    <t>LEMONADE</t>
+  </si>
+  <si>
+    <t>MASTERCARD</t>
+  </si>
+  <si>
+    <t>MICROCHIP</t>
+  </si>
+  <si>
+    <t>MARVELL</t>
+  </si>
+  <si>
+    <t>MORGAN_STANLEY</t>
+  </si>
+  <si>
+    <t>MICROSOFT</t>
+  </si>
+  <si>
+    <t>NETFLIX</t>
+  </si>
+  <si>
+    <t>NIKE</t>
+  </si>
+  <si>
+    <t>Service_Now</t>
+  </si>
+  <si>
+    <t>NUCOR</t>
+  </si>
+  <si>
+    <t>NVIDIA</t>
+  </si>
+  <si>
+    <t>NVE</t>
+  </si>
+  <si>
+    <t>REALTY_INCOME</t>
+  </si>
+  <si>
+    <t>ORACLE</t>
+  </si>
+  <si>
+    <t>PALO_ALTO</t>
+  </si>
+  <si>
+    <t>UIPATH</t>
+  </si>
+  <si>
+    <t>PROCTER_GAMBLE</t>
+  </si>
+  <si>
+    <t>PAYPAL</t>
+  </si>
+  <si>
+    <t>QUALCOMM</t>
+  </si>
+  <si>
+    <t>ROBLOX</t>
+  </si>
+  <si>
+    <t>STARBUCKS</t>
+  </si>
+  <si>
+    <t>SHOPIFY</t>
+  </si>
+  <si>
+    <t>SNOWFLAKE</t>
+  </si>
+  <si>
+    <t>SPLUNK</t>
+  </si>
+  <si>
+    <t>SQUARE_BLOCK</t>
+  </si>
+  <si>
+    <t>CONSTELLATION_BRANDS</t>
+  </si>
+  <si>
+    <t>SKYWORKS</t>
+  </si>
+  <si>
+    <t>TELADOC</t>
+  </si>
+  <si>
+    <t>ATLASSIAN</t>
+  </si>
+  <si>
+    <t>TESLA</t>
+  </si>
+  <si>
+    <t>TAIWAN_SEMICONDUCTOR</t>
+  </si>
+  <si>
+    <t>VISA</t>
+  </si>
+  <si>
+    <t>VERIZON</t>
+  </si>
+  <si>
+    <t>WALMART</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +475,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,9 +503,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,17 +790,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="200" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -434,6 +843,566 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B47" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>39</v>
+      </c>
+      <c r="B54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>18</v>
+      </c>
+      <c r="B58" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>50</v>
+      </c>
+      <c r="B63" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>41</v>
+      </c>
+      <c r="B64" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>55</v>
+      </c>
+      <c r="B68" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>43</v>
+      </c>
+      <c r="B69" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>52</v>
+      </c>
+      <c r="B70" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B71" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>49</v>
+      </c>
+      <c r="B72" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>40</v>
+      </c>
+      <c r="B75" t="s">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>